<commit_message>
add tools to manage close app matches
</commit_message>
<xml_diff>
--- a/Reports/ReviewedAppMatches.xlsx
+++ b/Reports/ReviewedAppMatches.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonathan Wise\Projects\webos-catalogutils\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonathan Wise\Projects\webos-catalog-utils\Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{97AEC6D7-86CB-4E97-92FB-1D65BE7F0CAB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{774F6263-7297-4897-98C2-951F793A7093}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{69250280-1989-40CE-B876-C325189B6CE8}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="596">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="595">
   <si>
     <t>App Name</t>
   </si>
@@ -97,9 +97,6 @@
   </si>
   <si>
     <t>com.ekesqueaky.animalabcs_1.1.1_all.ipk</t>
-  </si>
-  <si>
-    <t>com.ekesqueaky.animalabcs_1.0.0.ipk</t>
   </si>
   <si>
     <t>com.ekesqueaky.animalabcs_1.0.1_all.ipk</t>
@@ -2188,7 +2185,7 @@
   <dimension ref="A1:G179"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C179" sqref="C179"/>
+      <selection activeCell="C179" sqref="A1:C179"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2275,11 +2272,12 @@
         <v>19</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>21</v>
-      </c>
+      <c r="E7" s="1"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
@@ -2289,2066 +2287,2067 @@
         <v>23</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>26</v>
-      </c>
+      <c r="E8" s="1"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" t="s">
         <v>27</v>
-      </c>
-      <c r="B9" t="s">
-        <v>28</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>29</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>30</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="E9" s="1"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" t="s">
         <v>31</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G10" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="G10" s="3"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" t="s">
         <v>37</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" t="s">
         <v>40</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" t="s">
         <v>43</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" t="s">
         <v>46</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" s="3" t="s">
         <v>47</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
+        <v>48</v>
+      </c>
+      <c r="B15" t="s">
         <v>49</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
+        <v>51</v>
+      </c>
+      <c r="B16" t="s">
         <v>52</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E16" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
+        <v>56</v>
+      </c>
+      <c r="B17" t="s">
         <v>57</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
+        <v>59</v>
+      </c>
+      <c r="B18" t="s">
         <v>60</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
+        <v>62</v>
+      </c>
+      <c r="B19" t="s">
         <v>63</v>
-      </c>
-      <c r="B19" t="s">
-        <v>64</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>65</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
+        <v>66</v>
+      </c>
+      <c r="B20" t="s">
         <v>67</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
+        <v>69</v>
+      </c>
+      <c r="B21" t="s">
         <v>70</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
+        <v>72</v>
+      </c>
+      <c r="B22" t="s">
         <v>73</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" s="2" t="s">
         <v>74</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
+        <v>75</v>
+      </c>
+      <c r="B23" t="s">
         <v>76</v>
-      </c>
-      <c r="B23" t="s">
-        <v>77</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>78</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
+        <v>79</v>
+      </c>
+      <c r="B24" t="s">
         <v>80</v>
-      </c>
-      <c r="B24" t="s">
-        <v>81</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>82</v>
       </c>
       <c r="D24" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E24" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
+        <v>84</v>
+      </c>
+      <c r="B25" t="s">
         <v>85</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
+        <v>87</v>
+      </c>
+      <c r="B26" t="s">
         <v>88</v>
       </c>
-      <c r="B26" t="s">
+      <c r="C26" s="1" t="s">
         <v>89</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
+        <v>90</v>
+      </c>
+      <c r="B27" t="s">
         <v>91</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
+        <v>93</v>
+      </c>
+      <c r="B28" t="s">
         <v>94</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C28" s="1" t="s">
         <v>95</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
+        <v>96</v>
+      </c>
+      <c r="B29" t="s">
         <v>97</v>
       </c>
-      <c r="B29" t="s">
+      <c r="C29" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="D29" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="D29" s="1" t="s">
+      <c r="E29" s="1" t="s">
         <v>100</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
+        <v>101</v>
+      </c>
+      <c r="B30" t="s">
         <v>102</v>
       </c>
-      <c r="B30" t="s">
+      <c r="C30" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F30" s="1" t="s">
         <v>103</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
+        <v>107</v>
+      </c>
+      <c r="B31" t="s">
         <v>108</v>
       </c>
-      <c r="B31" t="s">
+      <c r="C31" s="1" t="s">
         <v>109</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
+        <v>110</v>
+      </c>
+      <c r="B32" t="s">
         <v>111</v>
       </c>
-      <c r="B32" t="s">
+      <c r="C32" s="1" t="s">
         <v>112</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
+        <v>113</v>
+      </c>
+      <c r="B33" t="s">
         <v>114</v>
       </c>
-      <c r="B33" t="s">
+      <c r="C33" s="1" t="s">
         <v>115</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
+        <v>116</v>
+      </c>
+      <c r="B34" t="s">
         <v>117</v>
-      </c>
-      <c r="B34" t="s">
-        <v>118</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>119</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
+        <v>120</v>
+      </c>
+      <c r="B35" t="s">
         <v>121</v>
       </c>
-      <c r="B35" t="s">
+      <c r="C35" s="1" t="s">
         <v>122</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
+        <v>123</v>
+      </c>
+      <c r="B36" t="s">
         <v>124</v>
       </c>
-      <c r="B36" t="s">
+      <c r="C36" s="1" t="s">
         <v>125</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
+        <v>126</v>
+      </c>
+      <c r="B37" t="s">
         <v>127</v>
       </c>
-      <c r="B37" t="s">
+      <c r="C37" s="1" t="s">
         <v>128</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
+        <v>129</v>
+      </c>
+      <c r="B38" t="s">
         <v>130</v>
       </c>
-      <c r="B38" t="s">
+      <c r="C38" s="2" t="s">
         <v>131</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
+        <v>132</v>
+      </c>
+      <c r="B39" t="s">
         <v>133</v>
       </c>
-      <c r="B39" t="s">
+      <c r="C39" s="3" t="s">
         <v>134</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
+        <v>135</v>
+      </c>
+      <c r="B40" t="s">
         <v>136</v>
-      </c>
-      <c r="B40" t="s">
-        <v>137</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>138</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
+        <v>139</v>
+      </c>
+      <c r="B41" t="s">
         <v>140</v>
       </c>
-      <c r="B41" t="s">
+      <c r="C41" s="2" t="s">
         <v>141</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
+        <v>142</v>
+      </c>
+      <c r="B42" t="s">
         <v>143</v>
-      </c>
-      <c r="B42" t="s">
-        <v>144</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>145</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
+        <v>146</v>
+      </c>
+      <c r="B43" t="s">
         <v>147</v>
       </c>
-      <c r="B43" t="s">
+      <c r="C43" s="1" t="s">
         <v>148</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
+        <v>149</v>
+      </c>
+      <c r="B44" t="s">
         <v>150</v>
       </c>
-      <c r="B44" t="s">
+      <c r="C44" s="1" t="s">
         <v>151</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
+        <v>152</v>
+      </c>
+      <c r="B45" t="s">
         <v>153</v>
-      </c>
-      <c r="B45" t="s">
-        <v>154</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>155</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
+        <v>156</v>
+      </c>
+      <c r="B46" t="s">
         <v>157</v>
       </c>
-      <c r="B46" t="s">
+      <c r="C46" s="1" t="s">
         <v>158</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
+        <v>159</v>
+      </c>
+      <c r="B47" t="s">
         <v>160</v>
       </c>
-      <c r="B47" t="s">
+      <c r="C47" s="1" t="s">
         <v>161</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
+        <v>162</v>
+      </c>
+      <c r="B48" t="s">
         <v>163</v>
       </c>
-      <c r="B48" t="s">
+      <c r="C48" s="1" t="s">
         <v>164</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
+        <v>165</v>
+      </c>
+      <c r="B49" t="s">
         <v>166</v>
       </c>
-      <c r="B49" t="s">
+      <c r="C49" s="1" t="s">
         <v>167</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
+        <v>168</v>
+      </c>
+      <c r="B50" t="s">
         <v>169</v>
-      </c>
-      <c r="B50" t="s">
-        <v>170</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>171</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
+        <v>172</v>
+      </c>
+      <c r="B51" t="s">
         <v>173</v>
       </c>
-      <c r="B51" t="s">
+      <c r="C51" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="G51" s="1" t="s">
         <v>174</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="F51" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="G51" s="1" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
+        <v>179</v>
+      </c>
+      <c r="B52" t="s">
         <v>180</v>
-      </c>
-      <c r="B52" t="s">
-        <v>181</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>182</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
+        <v>183</v>
+      </c>
+      <c r="B53" t="s">
         <v>184</v>
       </c>
-      <c r="B53" t="s">
+      <c r="C53" s="1" t="s">
         <v>185</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
+        <v>186</v>
+      </c>
+      <c r="B54" t="s">
         <v>187</v>
       </c>
-      <c r="B54" t="s">
+      <c r="C54" s="1" t="s">
         <v>188</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
+        <v>189</v>
+      </c>
+      <c r="B55" t="s">
         <v>190</v>
       </c>
-      <c r="B55" t="s">
+      <c r="C55" s="1" t="s">
         <v>191</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
+        <v>192</v>
+      </c>
+      <c r="B56" t="s">
         <v>193</v>
-      </c>
-      <c r="B56" t="s">
-        <v>194</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>195</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
+        <v>196</v>
+      </c>
+      <c r="B57" t="s">
         <v>197</v>
       </c>
-      <c r="B57" t="s">
+      <c r="C57" s="1" t="s">
         <v>198</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
+        <v>199</v>
+      </c>
+      <c r="B58" t="s">
         <v>200</v>
       </c>
-      <c r="B58" t="s">
+      <c r="C58" s="1" t="s">
         <v>201</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
+        <v>202</v>
+      </c>
+      <c r="B59" t="s">
         <v>203</v>
       </c>
-      <c r="B59" t="s">
+      <c r="C59" s="1" t="s">
         <v>204</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
+        <v>205</v>
+      </c>
+      <c r="B60" t="s">
         <v>206</v>
       </c>
-      <c r="B60" t="s">
+      <c r="C60" s="1" t="s">
         <v>207</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
+        <v>208</v>
+      </c>
+      <c r="B61" t="s">
         <v>209</v>
       </c>
-      <c r="B61" t="s">
+      <c r="C61" s="1" t="s">
         <v>210</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
+        <v>211</v>
+      </c>
+      <c r="B62" t="s">
         <v>212</v>
       </c>
-      <c r="B62" t="s">
+      <c r="C62" s="1" t="s">
         <v>213</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
+        <v>214</v>
+      </c>
+      <c r="B63" t="s">
         <v>215</v>
       </c>
-      <c r="B63" t="s">
+      <c r="C63" s="1" t="s">
         <v>216</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
+        <v>217</v>
+      </c>
+      <c r="B64" t="s">
         <v>218</v>
       </c>
-      <c r="B64" t="s">
+      <c r="C64" s="1" t="s">
         <v>219</v>
-      </c>
-      <c r="C64" s="1" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
+        <v>220</v>
+      </c>
+      <c r="B65" t="s">
         <v>221</v>
       </c>
-      <c r="B65" t="s">
+      <c r="C65" s="1" t="s">
         <v>222</v>
-      </c>
-      <c r="C65" s="1" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
+        <v>223</v>
+      </c>
+      <c r="B66" t="s">
         <v>224</v>
       </c>
-      <c r="B66" t="s">
+      <c r="C66" s="1" t="s">
         <v>225</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
+        <v>226</v>
+      </c>
+      <c r="B67" t="s">
         <v>227</v>
       </c>
-      <c r="B67" t="s">
+      <c r="C67" s="1" t="s">
         <v>228</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
+        <v>229</v>
+      </c>
+      <c r="B68" t="s">
         <v>230</v>
       </c>
-      <c r="B68" t="s">
+      <c r="C68" s="1" t="s">
         <v>231</v>
-      </c>
-      <c r="C68" s="1" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
+        <v>232</v>
+      </c>
+      <c r="B69" t="s">
         <v>233</v>
       </c>
-      <c r="B69" t="s">
+      <c r="C69" s="1" t="s">
         <v>234</v>
-      </c>
-      <c r="C69" s="1" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
+        <v>235</v>
+      </c>
+      <c r="B70" t="s">
         <v>236</v>
-      </c>
-      <c r="B70" t="s">
-        <v>237</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>238</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
+        <v>239</v>
+      </c>
+      <c r="B71" t="s">
         <v>240</v>
       </c>
-      <c r="B71" t="s">
+      <c r="C71" s="1" t="s">
         <v>241</v>
-      </c>
-      <c r="C71" s="1" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
+        <v>242</v>
+      </c>
+      <c r="B72" t="s">
         <v>243</v>
       </c>
-      <c r="B72" t="s">
+      <c r="C72" s="1" t="s">
         <v>244</v>
-      </c>
-      <c r="C72" s="1" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
+        <v>245</v>
+      </c>
+      <c r="B73" t="s">
         <v>246</v>
-      </c>
-      <c r="B73" t="s">
-        <v>247</v>
       </c>
       <c r="C73" s="1" t="s">
         <v>248</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
+        <v>249</v>
+      </c>
+      <c r="B74" t="s">
         <v>250</v>
       </c>
-      <c r="B74" t="s">
+      <c r="C74" s="2" t="s">
         <v>251</v>
-      </c>
-      <c r="C74" s="2" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
+        <v>252</v>
+      </c>
+      <c r="B75" t="s">
         <v>253</v>
       </c>
-      <c r="B75" t="s">
+      <c r="C75" s="1" t="s">
         <v>254</v>
-      </c>
-      <c r="C75" s="1" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
+        <v>255</v>
+      </c>
+      <c r="B76" t="s">
         <v>256</v>
       </c>
-      <c r="B76" t="s">
+      <c r="C76" s="1" t="s">
         <v>257</v>
-      </c>
-      <c r="C76" s="1" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
+        <v>258</v>
+      </c>
+      <c r="B77" t="s">
         <v>259</v>
       </c>
-      <c r="B77" t="s">
+      <c r="C77" s="1" t="s">
         <v>260</v>
-      </c>
-      <c r="C77" s="1" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
+        <v>261</v>
+      </c>
+      <c r="B78" t="s">
         <v>262</v>
       </c>
-      <c r="B78" t="s">
+      <c r="C78" s="2" t="s">
         <v>263</v>
-      </c>
-      <c r="C78" s="2" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
+        <v>264</v>
+      </c>
+      <c r="B79" t="s">
         <v>265</v>
       </c>
-      <c r="B79" t="s">
+      <c r="C79" s="1" t="s">
         <v>266</v>
-      </c>
-      <c r="C79" s="1" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
+        <v>267</v>
+      </c>
+      <c r="B80" t="s">
         <v>268</v>
       </c>
-      <c r="B80" t="s">
+      <c r="C80" s="1" t="s">
         <v>269</v>
-      </c>
-      <c r="C80" s="1" t="s">
-        <v>270</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
+        <v>270</v>
+      </c>
+      <c r="B81" t="s">
         <v>271</v>
       </c>
-      <c r="B81" t="s">
+      <c r="C81" s="1" t="s">
         <v>272</v>
-      </c>
-      <c r="C81" s="1" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
+        <v>273</v>
+      </c>
+      <c r="B82" t="s">
         <v>274</v>
       </c>
-      <c r="B82" t="s">
+      <c r="C82" s="1" t="s">
         <v>275</v>
-      </c>
-      <c r="C82" s="1" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
+        <v>276</v>
+      </c>
+      <c r="B83" t="s">
         <v>277</v>
       </c>
-      <c r="B83" t="s">
+      <c r="C83" s="1" t="s">
         <v>278</v>
-      </c>
-      <c r="C83" s="1" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
+        <v>279</v>
+      </c>
+      <c r="B84" t="s">
         <v>280</v>
       </c>
-      <c r="B84" t="s">
+      <c r="C84" s="2" t="s">
         <v>281</v>
-      </c>
-      <c r="C84" s="2" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
+        <v>282</v>
+      </c>
+      <c r="B85" t="s">
         <v>283</v>
       </c>
-      <c r="B85" t="s">
+      <c r="C85" s="1" t="s">
         <v>284</v>
-      </c>
-      <c r="C85" s="1" t="s">
-        <v>285</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
+        <v>285</v>
+      </c>
+      <c r="B86" t="s">
         <v>286</v>
       </c>
-      <c r="B86" t="s">
+      <c r="C86" s="1" t="s">
         <v>287</v>
-      </c>
-      <c r="C86" s="1" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
+        <v>288</v>
+      </c>
+      <c r="B87" t="s">
         <v>289</v>
       </c>
-      <c r="B87" t="s">
+      <c r="C87" s="1" t="s">
         <v>290</v>
-      </c>
-      <c r="C87" s="1" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
+        <v>291</v>
+      </c>
+      <c r="B88" t="s">
         <v>292</v>
       </c>
-      <c r="B88" t="s">
+      <c r="C88" s="1" t="s">
         <v>293</v>
-      </c>
-      <c r="C88" s="1" t="s">
-        <v>294</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
+        <v>294</v>
+      </c>
+      <c r="B89" t="s">
         <v>295</v>
       </c>
-      <c r="B89" t="s">
+      <c r="C89" s="1" t="s">
         <v>296</v>
-      </c>
-      <c r="C89" s="1" t="s">
-        <v>297</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
+        <v>297</v>
+      </c>
+      <c r="B90" t="s">
         <v>298</v>
       </c>
-      <c r="B90" t="s">
+      <c r="C90" s="2" t="s">
         <v>299</v>
-      </c>
-      <c r="C90" s="2" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
+        <v>300</v>
+      </c>
+      <c r="B91" t="s">
         <v>301</v>
       </c>
-      <c r="B91" t="s">
+      <c r="C91" s="1" t="s">
         <v>302</v>
-      </c>
-      <c r="C91" s="1" t="s">
-        <v>303</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
+        <v>303</v>
+      </c>
+      <c r="B92" t="s">
         <v>304</v>
       </c>
-      <c r="B92" t="s">
+      <c r="C92" s="1" t="s">
         <v>305</v>
-      </c>
-      <c r="C92" s="1" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
+        <v>306</v>
+      </c>
+      <c r="B93" t="s">
         <v>307</v>
       </c>
-      <c r="B93" t="s">
+      <c r="C93" s="1" t="s">
         <v>308</v>
-      </c>
-      <c r="C93" s="1" t="s">
-        <v>309</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
+        <v>309</v>
+      </c>
+      <c r="B94" t="s">
         <v>310</v>
       </c>
-      <c r="B94" t="s">
+      <c r="C94" s="1" t="s">
         <v>311</v>
-      </c>
-      <c r="C94" s="1" t="s">
-        <v>312</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
+        <v>312</v>
+      </c>
+      <c r="B95" t="s">
         <v>313</v>
       </c>
-      <c r="B95" t="s">
+      <c r="C95" s="1" t="s">
         <v>314</v>
-      </c>
-      <c r="C95" s="1" t="s">
-        <v>315</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
+        <v>315</v>
+      </c>
+      <c r="B96" t="s">
         <v>316</v>
       </c>
-      <c r="B96" t="s">
+      <c r="C96" s="1" t="s">
         <v>317</v>
-      </c>
-      <c r="C96" s="1" t="s">
-        <v>318</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
+        <v>318</v>
+      </c>
+      <c r="B97" t="s">
         <v>319</v>
       </c>
-      <c r="B97" t="s">
+      <c r="C97" s="1" t="s">
         <v>320</v>
-      </c>
-      <c r="C97" s="1" t="s">
-        <v>321</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
+        <v>321</v>
+      </c>
+      <c r="B98" t="s">
         <v>322</v>
       </c>
-      <c r="B98" t="s">
+      <c r="C98" s="1" t="s">
         <v>323</v>
-      </c>
-      <c r="C98" s="1" t="s">
-        <v>324</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
+        <v>324</v>
+      </c>
+      <c r="B99" t="s">
         <v>325</v>
       </c>
-      <c r="B99" t="s">
-        <v>326</v>
-      </c>
       <c r="C99" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
+        <v>326</v>
+      </c>
+      <c r="B100" t="s">
         <v>327</v>
       </c>
-      <c r="B100" t="s">
+      <c r="C100" s="1" t="s">
         <v>328</v>
-      </c>
-      <c r="C100" s="1" t="s">
-        <v>329</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
+        <v>329</v>
+      </c>
+      <c r="B101" t="s">
         <v>330</v>
       </c>
-      <c r="B101" t="s">
+      <c r="C101" s="1" t="s">
         <v>331</v>
-      </c>
-      <c r="C101" s="1" t="s">
-        <v>332</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
+        <v>332</v>
+      </c>
+      <c r="B102" t="s">
         <v>333</v>
       </c>
-      <c r="B102" t="s">
+      <c r="C102" s="1" t="s">
         <v>334</v>
-      </c>
-      <c r="C102" s="1" t="s">
-        <v>335</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
+        <v>335</v>
+      </c>
+      <c r="B103" t="s">
         <v>336</v>
       </c>
-      <c r="B103" t="s">
+      <c r="C103" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="D103" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="E103" s="1" t="s">
         <v>337</v>
-      </c>
-      <c r="C103" s="1" t="s">
-        <v>338</v>
-      </c>
-      <c r="D103" s="1" t="s">
-        <v>339</v>
-      </c>
-      <c r="E103" s="1" t="s">
-        <v>340</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
+        <v>340</v>
+      </c>
+      <c r="B104" t="s">
         <v>341</v>
       </c>
-      <c r="B104" t="s">
+      <c r="C104" s="1" t="s">
         <v>342</v>
-      </c>
-      <c r="C104" s="1" t="s">
-        <v>343</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
+        <v>343</v>
+      </c>
+      <c r="B105" t="s">
         <v>344</v>
       </c>
-      <c r="B105" t="s">
+      <c r="C105" s="1" t="s">
         <v>345</v>
-      </c>
-      <c r="C105" s="1" t="s">
-        <v>346</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
+        <v>346</v>
+      </c>
+      <c r="B106" t="s">
         <v>347</v>
       </c>
-      <c r="B106" t="s">
+      <c r="C106" s="2" t="s">
         <v>348</v>
-      </c>
-      <c r="C106" s="2" t="s">
-        <v>349</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
+        <v>349</v>
+      </c>
+      <c r="B107" t="s">
         <v>350</v>
       </c>
-      <c r="B107" t="s">
+      <c r="C107" s="2" t="s">
         <v>351</v>
-      </c>
-      <c r="C107" s="2" t="s">
-        <v>352</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
+        <v>352</v>
+      </c>
+      <c r="B108" t="s">
         <v>353</v>
       </c>
-      <c r="B108" t="s">
+      <c r="C108" s="1" t="s">
         <v>354</v>
-      </c>
-      <c r="C108" s="1" t="s">
-        <v>355</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
+        <v>355</v>
+      </c>
+      <c r="B109" t="s">
         <v>356</v>
       </c>
-      <c r="B109" t="s">
+      <c r="C109" s="1" t="s">
         <v>357</v>
-      </c>
-      <c r="C109" s="1" t="s">
-        <v>358</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
+        <v>358</v>
+      </c>
+      <c r="B110" t="s">
         <v>359</v>
       </c>
-      <c r="B110" t="s">
+      <c r="C110" s="1" t="s">
         <v>360</v>
-      </c>
-      <c r="C110" s="1" t="s">
-        <v>361</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
+        <v>361</v>
+      </c>
+      <c r="B111" t="s">
         <v>362</v>
       </c>
-      <c r="B111" t="s">
+      <c r="C111" s="1" t="s">
         <v>363</v>
-      </c>
-      <c r="C111" s="1" t="s">
-        <v>364</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
+        <v>364</v>
+      </c>
+      <c r="B112" t="s">
         <v>365</v>
       </c>
-      <c r="B112" t="s">
+      <c r="C112" s="1" t="s">
         <v>366</v>
-      </c>
-      <c r="C112" s="1" t="s">
-        <v>367</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
+        <v>367</v>
+      </c>
+      <c r="B113" t="s">
         <v>368</v>
       </c>
-      <c r="B113" t="s">
+      <c r="C113" s="1" t="s">
         <v>369</v>
-      </c>
-      <c r="C113" s="1" t="s">
-        <v>370</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
+        <v>370</v>
+      </c>
+      <c r="B114" t="s">
         <v>371</v>
       </c>
-      <c r="B114" t="s">
+      <c r="C114" s="2" t="s">
         <v>372</v>
-      </c>
-      <c r="C114" s="2" t="s">
-        <v>373</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
+        <v>373</v>
+      </c>
+      <c r="B115" t="s">
         <v>374</v>
       </c>
-      <c r="B115" t="s">
+      <c r="C115" s="1" t="s">
         <v>375</v>
-      </c>
-      <c r="C115" s="1" t="s">
-        <v>376</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
+        <v>376</v>
+      </c>
+      <c r="B116" t="s">
         <v>377</v>
       </c>
-      <c r="B116" t="s">
+      <c r="C116" s="1" t="s">
         <v>378</v>
-      </c>
-      <c r="C116" s="1" t="s">
-        <v>379</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
+        <v>379</v>
+      </c>
+      <c r="B117" t="s">
         <v>380</v>
       </c>
-      <c r="B117" t="s">
+      <c r="C117" s="1" t="s">
         <v>381</v>
       </c>
-      <c r="C117" s="1" t="s">
+      <c r="D117" s="1" t="s">
         <v>382</v>
-      </c>
-      <c r="D117" s="1" t="s">
-        <v>383</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
+        <v>383</v>
+      </c>
+      <c r="B118" t="s">
         <v>384</v>
       </c>
-      <c r="B118" t="s">
+      <c r="C118" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="D118" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="E118" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="F118" s="1" t="s">
         <v>385</v>
-      </c>
-      <c r="C118" s="1" t="s">
-        <v>386</v>
-      </c>
-      <c r="D118" s="1" t="s">
-        <v>387</v>
-      </c>
-      <c r="E118" s="1" t="s">
-        <v>388</v>
-      </c>
-      <c r="F118" s="1" t="s">
-        <v>389</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
+        <v>389</v>
+      </c>
+      <c r="B119" t="s">
         <v>390</v>
       </c>
-      <c r="B119" t="s">
+      <c r="C119" s="1" t="s">
         <v>391</v>
       </c>
-      <c r="C119" s="1" t="s">
+      <c r="D119" s="1" t="s">
         <v>392</v>
-      </c>
-      <c r="D119" s="1" t="s">
-        <v>393</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
+        <v>393</v>
+      </c>
+      <c r="B120" t="s">
         <v>394</v>
       </c>
-      <c r="B120" t="s">
+      <c r="C120" s="1" t="s">
         <v>395</v>
-      </c>
-      <c r="C120" s="1" t="s">
-        <v>396</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
+        <v>396</v>
+      </c>
+      <c r="B121" t="s">
         <v>397</v>
-      </c>
-      <c r="B121" t="s">
-        <v>398</v>
       </c>
       <c r="C121" s="1" t="s">
         <v>399</v>
       </c>
       <c r="D121" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="E121" s="1" t="s">
         <v>400</v>
       </c>
-      <c r="E121" s="1" t="s">
+      <c r="F121" s="1" t="s">
         <v>401</v>
-      </c>
-      <c r="F121" s="1" t="s">
-        <v>402</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
+        <v>402</v>
+      </c>
+      <c r="B122" t="s">
         <v>403</v>
       </c>
-      <c r="B122" t="s">
+      <c r="C122" s="3" t="s">
         <v>404</v>
-      </c>
-      <c r="C122" s="3" t="s">
-        <v>405</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
+        <v>405</v>
+      </c>
+      <c r="B123" t="s">
         <v>406</v>
       </c>
-      <c r="B123" t="s">
+      <c r="C123" s="1" t="s">
         <v>407</v>
-      </c>
-      <c r="C123" s="1" t="s">
-        <v>408</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
+        <v>408</v>
+      </c>
+      <c r="B124" t="s">
         <v>409</v>
       </c>
-      <c r="B124" t="s">
+      <c r="C124" s="1" t="s">
         <v>410</v>
-      </c>
-      <c r="C124" s="1" t="s">
-        <v>411</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
+        <v>411</v>
+      </c>
+      <c r="B125" t="s">
         <v>412</v>
       </c>
-      <c r="B125" t="s">
+      <c r="C125" s="1" t="s">
         <v>413</v>
-      </c>
-      <c r="C125" s="1" t="s">
-        <v>414</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
+        <v>414</v>
+      </c>
+      <c r="B126" t="s">
         <v>415</v>
       </c>
-      <c r="B126" t="s">
+      <c r="C126" s="1" t="s">
         <v>416</v>
-      </c>
-      <c r="C126" s="1" t="s">
-        <v>417</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
+        <v>417</v>
+      </c>
+      <c r="B127" t="s">
         <v>418</v>
       </c>
-      <c r="B127" t="s">
+      <c r="C127" s="1" t="s">
         <v>419</v>
-      </c>
-      <c r="C127" s="1" t="s">
-        <v>420</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
+        <v>420</v>
+      </c>
+      <c r="B128" t="s">
         <v>421</v>
       </c>
-      <c r="B128" t="s">
+      <c r="C128" s="1" t="s">
         <v>422</v>
       </c>
-      <c r="C128" s="1" t="s">
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A129" t="s">
         <v>423</v>
       </c>
-    </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A129" t="s">
+      <c r="B129" t="s">
         <v>424</v>
       </c>
-      <c r="B129" t="s">
+      <c r="C129" s="2" t="s">
+        <v>427</v>
+      </c>
+      <c r="D129" s="2" t="s">
+        <v>426</v>
+      </c>
+      <c r="F129" s="1" t="s">
         <v>425</v>
       </c>
-      <c r="C129" s="1" t="s">
-        <v>426</v>
-      </c>
-      <c r="D129" s="2" t="s">
-        <v>427</v>
-      </c>
-      <c r="E129" s="2" t="s">
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A130" t="s">
         <v>428</v>
       </c>
-    </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A130" t="s">
+      <c r="B130" t="s">
         <v>429</v>
       </c>
-      <c r="B130" t="s">
+      <c r="C130" s="1" t="s">
         <v>430</v>
       </c>
-      <c r="C130" s="1" t="s">
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A131" t="s">
         <v>431</v>
       </c>
-    </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A131" t="s">
+      <c r="B131" t="s">
         <v>432</v>
-      </c>
-      <c r="B131" t="s">
-        <v>433</v>
       </c>
       <c r="C131" s="1" t="s">
         <v>434</v>
       </c>
       <c r="D131" s="1" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A132" t="s">
         <v>435</v>
       </c>
-    </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A132" t="s">
+      <c r="B132" t="s">
         <v>436</v>
-      </c>
-      <c r="B132" t="s">
-        <v>437</v>
       </c>
       <c r="C132" s="1" t="s">
         <v>438</v>
       </c>
       <c r="D132" s="1" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A133" t="s">
         <v>439</v>
       </c>
-    </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A133" t="s">
+      <c r="B133" t="s">
         <v>440</v>
       </c>
-      <c r="B133" t="s">
+      <c r="C133" s="1" t="s">
         <v>441</v>
       </c>
-      <c r="C133" s="1" t="s">
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A134" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A134" t="s">
+      <c r="B134" t="s">
         <v>443</v>
       </c>
-      <c r="B134" t="s">
+      <c r="C134" s="1" t="s">
         <v>444</v>
       </c>
-      <c r="C134" s="1" t="s">
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A135" t="s">
         <v>445</v>
       </c>
-    </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A135" t="s">
+      <c r="B135" t="s">
         <v>446</v>
       </c>
-      <c r="B135" t="s">
+      <c r="C135" s="1" t="s">
         <v>447</v>
       </c>
-      <c r="C135" s="1" t="s">
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A136" t="s">
         <v>448</v>
       </c>
-    </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A136" t="s">
+      <c r="B136" t="s">
         <v>449</v>
       </c>
-      <c r="B136" t="s">
+      <c r="C136" s="1" t="s">
         <v>450</v>
       </c>
-      <c r="C136" s="1" t="s">
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A137" t="s">
         <v>451</v>
       </c>
-    </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A137" t="s">
+      <c r="B137" t="s">
         <v>452</v>
       </c>
-      <c r="B137" t="s">
+      <c r="C137" s="1" t="s">
         <v>453</v>
       </c>
-      <c r="C137" s="1" t="s">
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A138" t="s">
         <v>454</v>
       </c>
-    </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A138" t="s">
+      <c r="B138" t="s">
         <v>455</v>
       </c>
-      <c r="B138" t="s">
+      <c r="C138" s="1" t="s">
         <v>456</v>
       </c>
-      <c r="C138" s="1" t="s">
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A139" t="s">
         <v>457</v>
       </c>
-    </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A139" t="s">
+      <c r="B139" t="s">
         <v>458</v>
       </c>
-      <c r="B139" t="s">
+      <c r="C139" s="1" t="s">
         <v>459</v>
       </c>
-      <c r="C139" s="1" t="s">
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A140" t="s">
         <v>460</v>
       </c>
-    </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A140" t="s">
+      <c r="B140" t="s">
         <v>461</v>
       </c>
-      <c r="B140" t="s">
+      <c r="C140" s="1" t="s">
         <v>462</v>
       </c>
-      <c r="C140" s="1" t="s">
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A141" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A141" t="s">
+      <c r="B141" t="s">
         <v>464</v>
       </c>
-      <c r="B141" t="s">
+      <c r="C141" s="1" t="s">
         <v>465</v>
       </c>
-      <c r="C141" s="1" t="s">
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A142" t="s">
         <v>466</v>
       </c>
-    </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A142" t="s">
+      <c r="B142" t="s">
         <v>467</v>
       </c>
-      <c r="B142" t="s">
+      <c r="C142" s="1" t="s">
+        <v>470</v>
+      </c>
+      <c r="D142" s="1" t="s">
+        <v>469</v>
+      </c>
+      <c r="E142" s="1" t="s">
         <v>468</v>
       </c>
-      <c r="C142" s="1" t="s">
-        <v>469</v>
-      </c>
-      <c r="D142" s="1" t="s">
-        <v>470</v>
-      </c>
-      <c r="E142" s="1" t="s">
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A143" t="s">
         <v>471</v>
       </c>
-    </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A143" t="s">
+      <c r="B143" t="s">
         <v>472</v>
       </c>
-      <c r="B143" t="s">
+      <c r="C143" s="1" t="s">
         <v>473</v>
       </c>
-      <c r="C143" s="1" t="s">
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A144" t="s">
         <v>474</v>
       </c>
-    </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A144" t="s">
+      <c r="B144" t="s">
         <v>475</v>
       </c>
-      <c r="B144" t="s">
+      <c r="C144" s="1" t="s">
         <v>476</v>
-      </c>
-      <c r="C144" s="1" t="s">
-        <v>477</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
+        <v>477</v>
+      </c>
+      <c r="B145" t="s">
         <v>478</v>
       </c>
-      <c r="B145" t="s">
+      <c r="C145" s="1" t="s">
         <v>479</v>
-      </c>
-      <c r="C145" s="1" t="s">
-        <v>480</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
+        <v>480</v>
+      </c>
+      <c r="B146" t="s">
         <v>481</v>
       </c>
-      <c r="B146" t="s">
+      <c r="C146" s="1" t="s">
         <v>482</v>
-      </c>
-      <c r="C146" s="1" t="s">
-        <v>483</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
+        <v>483</v>
+      </c>
+      <c r="B147" t="s">
         <v>484</v>
       </c>
-      <c r="B147" t="s">
+      <c r="C147" s="1" t="s">
         <v>485</v>
-      </c>
-      <c r="C147" s="1" t="s">
-        <v>486</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
+        <v>486</v>
+      </c>
+      <c r="B148" t="s">
         <v>487</v>
       </c>
-      <c r="B148" t="s">
+      <c r="C148" s="1" t="s">
         <v>488</v>
-      </c>
-      <c r="C148" s="1" t="s">
-        <v>489</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
+        <v>489</v>
+      </c>
+      <c r="B149" t="s">
         <v>490</v>
       </c>
-      <c r="B149" t="s">
+      <c r="C149" s="1" t="s">
         <v>491</v>
-      </c>
-      <c r="C149" s="1" t="s">
-        <v>492</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
+        <v>492</v>
+      </c>
+      <c r="B150" t="s">
         <v>493</v>
       </c>
-      <c r="B150" t="s">
+      <c r="C150" s="1" t="s">
         <v>494</v>
-      </c>
-      <c r="C150" s="1" t="s">
-        <v>495</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
+        <v>495</v>
+      </c>
+      <c r="B151" t="s">
         <v>496</v>
       </c>
-      <c r="B151" t="s">
+      <c r="C151" s="1" t="s">
         <v>497</v>
-      </c>
-      <c r="C151" s="1" t="s">
-        <v>498</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
+        <v>498</v>
+      </c>
+      <c r="B152" t="s">
         <v>499</v>
       </c>
-      <c r="B152" t="s">
+      <c r="C152" s="1" t="s">
         <v>500</v>
-      </c>
-      <c r="C152" s="1" t="s">
-        <v>501</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
+        <v>501</v>
+      </c>
+      <c r="B153" t="s">
         <v>502</v>
       </c>
-      <c r="B153" t="s">
+      <c r="C153" s="1" t="s">
         <v>503</v>
-      </c>
-      <c r="C153" s="1" t="s">
-        <v>504</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
+        <v>504</v>
+      </c>
+      <c r="B154" t="s">
         <v>505</v>
       </c>
-      <c r="B154" t="s">
+      <c r="C154" s="1" t="s">
         <v>506</v>
-      </c>
-      <c r="C154" s="1" t="s">
-        <v>507</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
+        <v>507</v>
+      </c>
+      <c r="B155" t="s">
         <v>508</v>
       </c>
-      <c r="B155" t="s">
+      <c r="C155" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="D155" s="1" t="s">
+        <v>510</v>
+      </c>
+      <c r="E155" s="1" t="s">
         <v>509</v>
-      </c>
-      <c r="C155" s="1" t="s">
-        <v>510</v>
-      </c>
-      <c r="D155" s="1" t="s">
-        <v>511</v>
-      </c>
-      <c r="E155" s="1" t="s">
-        <v>512</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
+        <v>512</v>
+      </c>
+      <c r="B156" t="s">
         <v>513</v>
       </c>
-      <c r="B156" t="s">
+      <c r="C156" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="C156" s="1" t="s">
+      <c r="D156" s="1" t="s">
         <v>515</v>
-      </c>
-      <c r="D156" s="1" t="s">
-        <v>516</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
+        <v>516</v>
+      </c>
+      <c r="B157" t="s">
         <v>517</v>
       </c>
-      <c r="B157" t="s">
+      <c r="C157" s="2" t="s">
         <v>518</v>
-      </c>
-      <c r="C157" s="2" t="s">
-        <v>519</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
+        <v>519</v>
+      </c>
+      <c r="B158" t="s">
         <v>520</v>
       </c>
-      <c r="B158" t="s">
+      <c r="C158" s="1" t="s">
         <v>521</v>
-      </c>
-      <c r="C158" s="1" t="s">
-        <v>522</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
+        <v>522</v>
+      </c>
+      <c r="B159" t="s">
         <v>523</v>
       </c>
-      <c r="B159" t="s">
+      <c r="C159" s="1" t="s">
+        <v>526</v>
+      </c>
+      <c r="D159" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="E159" s="1" t="s">
         <v>524</v>
-      </c>
-      <c r="C159" s="1" t="s">
-        <v>525</v>
-      </c>
-      <c r="D159" s="1" t="s">
-        <v>526</v>
-      </c>
-      <c r="E159" s="1" t="s">
-        <v>527</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
+        <v>527</v>
+      </c>
+      <c r="B160" t="s">
         <v>528</v>
       </c>
-      <c r="B160" t="s">
+      <c r="C160" s="1" t="s">
         <v>529</v>
-      </c>
-      <c r="C160" s="1" t="s">
-        <v>530</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
+        <v>530</v>
+      </c>
+      <c r="B161" t="s">
         <v>531</v>
       </c>
-      <c r="B161" t="s">
+      <c r="C161" s="1" t="s">
         <v>532</v>
       </c>
-      <c r="C161" s="1" t="s">
+      <c r="D161" s="1" t="s">
         <v>533</v>
-      </c>
-      <c r="D161" s="1" t="s">
-        <v>534</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
+        <v>534</v>
+      </c>
+      <c r="B162" t="s">
         <v>535</v>
       </c>
-      <c r="B162" t="s">
+      <c r="C162" s="1" t="s">
         <v>536</v>
-      </c>
-      <c r="C162" s="1" t="s">
-        <v>537</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
+        <v>537</v>
+      </c>
+      <c r="B163" t="s">
         <v>538</v>
       </c>
-      <c r="B163" t="s">
+      <c r="C163" s="1" t="s">
         <v>539</v>
-      </c>
-      <c r="C163" s="1" t="s">
-        <v>540</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
+        <v>540</v>
+      </c>
+      <c r="B164" t="s">
         <v>541</v>
       </c>
-      <c r="B164" t="s">
+      <c r="C164" s="1" t="s">
         <v>542</v>
-      </c>
-      <c r="C164" s="1" t="s">
-        <v>543</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
+        <v>543</v>
+      </c>
+      <c r="B165" t="s">
         <v>544</v>
-      </c>
-      <c r="B165" t="s">
-        <v>545</v>
       </c>
       <c r="C165" s="1" t="s">
         <v>546</v>
       </c>
       <c r="D165" s="1" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
+        <v>547</v>
+      </c>
+      <c r="B166" t="s">
         <v>548</v>
       </c>
-      <c r="B166" t="s">
+      <c r="C166" s="1" t="s">
+        <v>551</v>
+      </c>
+      <c r="D166" s="1" t="s">
+        <v>550</v>
+      </c>
+      <c r="E166" s="1" t="s">
         <v>549</v>
-      </c>
-      <c r="C166" s="1" t="s">
-        <v>550</v>
-      </c>
-      <c r="D166" s="1" t="s">
-        <v>551</v>
-      </c>
-      <c r="E166" s="1" t="s">
-        <v>552</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
+        <v>552</v>
+      </c>
+      <c r="B167" t="s">
         <v>553</v>
       </c>
-      <c r="B167" t="s">
+      <c r="C167" s="2" t="s">
         <v>554</v>
-      </c>
-      <c r="C167" s="2" t="s">
-        <v>555</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
+        <v>555</v>
+      </c>
+      <c r="B168" t="s">
         <v>556</v>
       </c>
-      <c r="B168" t="s">
+      <c r="C168" s="1" t="s">
         <v>557</v>
-      </c>
-      <c r="C168" s="1" t="s">
-        <v>558</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
+        <v>558</v>
+      </c>
+      <c r="B169" t="s">
         <v>559</v>
-      </c>
-      <c r="B169" t="s">
-        <v>560</v>
       </c>
       <c r="C169" s="1" t="s">
         <v>561</v>
       </c>
       <c r="D169" s="1" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
+        <v>562</v>
+      </c>
+      <c r="B170" t="s">
         <v>563</v>
       </c>
-      <c r="B170" t="s">
+      <c r="C170" s="1" t="s">
         <v>564</v>
       </c>
-      <c r="C170" s="1" t="s">
+      <c r="D170" s="1" t="s">
         <v>565</v>
-      </c>
-      <c r="D170" s="1" t="s">
-        <v>566</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
+        <v>566</v>
+      </c>
+      <c r="B171" t="s">
         <v>567</v>
       </c>
-      <c r="B171" t="s">
+      <c r="C171" s="1" t="s">
         <v>568</v>
       </c>
-      <c r="C171" s="1" t="s">
+      <c r="D171" s="1" t="s">
         <v>569</v>
-      </c>
-      <c r="D171" s="1" t="s">
-        <v>570</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
+        <v>570</v>
+      </c>
+      <c r="B172" t="s">
         <v>571</v>
       </c>
-      <c r="B172" t="s">
+      <c r="C172" s="1" t="s">
         <v>572</v>
-      </c>
-      <c r="C172" s="1" t="s">
-        <v>573</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
+        <v>573</v>
+      </c>
+      <c r="B173" t="s">
         <v>574</v>
       </c>
-      <c r="B173" t="s">
+      <c r="C173" s="1" t="s">
         <v>575</v>
-      </c>
-      <c r="C173" s="1" t="s">
-        <v>576</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
+        <v>576</v>
+      </c>
+      <c r="B174" t="s">
         <v>577</v>
       </c>
-      <c r="B174" t="s">
+      <c r="C174" s="1" t="s">
         <v>578</v>
-      </c>
-      <c r="C174" s="1" t="s">
-        <v>579</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
+        <v>579</v>
+      </c>
+      <c r="B175" t="s">
         <v>580</v>
       </c>
-      <c r="B175" t="s">
+      <c r="C175" s="1" t="s">
         <v>581</v>
-      </c>
-      <c r="C175" s="1" t="s">
-        <v>582</v>
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
+        <v>582</v>
+      </c>
+      <c r="B176" t="s">
         <v>583</v>
       </c>
-      <c r="B176" t="s">
+      <c r="C176" s="1" t="s">
         <v>584</v>
-      </c>
-      <c r="C176" s="1" t="s">
-        <v>585</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
+        <v>585</v>
+      </c>
+      <c r="B177" t="s">
         <v>586</v>
       </c>
-      <c r="B177" t="s">
+      <c r="C177" s="1" t="s">
         <v>587</v>
-      </c>
-      <c r="C177" s="1" t="s">
-        <v>588</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
+        <v>588</v>
+      </c>
+      <c r="B178" t="s">
         <v>589</v>
-      </c>
-      <c r="B178" t="s">
-        <v>590</v>
       </c>
       <c r="C178" s="1" t="s">
         <v>591</v>
       </c>
       <c r="D178" s="1" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
+        <v>592</v>
+      </c>
+      <c r="B179" t="s">
         <v>593</v>
       </c>
-      <c r="B179" t="s">
+      <c r="C179" s="1" t="s">
         <v>594</v>
-      </c>
-      <c r="C179" s="1" t="s">
-        <v>595</v>
       </c>
     </row>
   </sheetData>

</xml_diff>